<commit_message>
genesis test results added to spread sheet
</commit_message>
<xml_diff>
--- a/Project 3 Genesis/Genesis Test Cases.xlsx
+++ b/Project 3 Genesis/Genesis Test Cases.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ndou\Documents\Sisekelo\Group3\Project 3 Genesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1864B2A1-C677-4E8A-9E19-C0E163938D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20325" windowHeight="9630"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="76">
   <si>
     <t>Test Case</t>
   </si>
@@ -150,9 +151,6 @@
   </si>
   <si>
     <t>1234,1 nov</t>
-  </si>
-  <si>
-    <t>It should show an error message that the field requires characters and a newer date</t>
   </si>
   <si>
     <t>Check if coupon field accepts a coupon that doesn’t exist</t>
@@ -205,13 +203,64 @@
   <si>
     <t xml:space="preserve">Enter 5 character on mobile number. Enter an existing email address peterntshuntsha24@gmail.com.  Click on the Register button.
 </t>
+  </si>
+  <si>
+    <t>Actual Resulsts</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>No Message was displayed</t>
+  </si>
+  <si>
+    <t>There are no links on related couses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It allowed user to enroll same course more than once </t>
+  </si>
+  <si>
+    <t>Itshows Error 404 page dosenot exist</t>
+  </si>
+  <si>
+    <t>It shows an error messages</t>
+  </si>
+  <si>
+    <t>it allows phone number to be letters [a-z/A-Z}</t>
+  </si>
+  <si>
+    <t>It allowes user to enter invalid email</t>
+  </si>
+  <si>
+    <t>It shows an error messages for password length</t>
+  </si>
+  <si>
+    <t>It allowed user to use numbers as first and last name</t>
+  </si>
+  <si>
+    <t>it allows zip code to be letters [a-z/A-Z}</t>
+  </si>
+  <si>
+    <t>It doesn’t send an email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It allowed user to request a call on date before today </t>
+  </si>
+  <si>
+    <t>It should show an error message that the field requires characters and a future date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -239,13 +288,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -261,7 +330,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
@@ -289,6 +358,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -570,11 +649,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,9 +664,11 @@
     <col min="4" max="4" width="56.5703125" style="4" customWidth="1"/>
     <col min="5" max="5" width="28" style="9" customWidth="1"/>
     <col min="6" max="6" width="56.85546875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="40.140625" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -606,8 +687,14 @@
       <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G1" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -618,7 +705,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>9</v>
@@ -626,8 +713,14 @@
       <c r="F2" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -646,8 +739,14 @@
       <c r="F3" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G3" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -666,8 +765,14 @@
       <c r="F4" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G4" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -686,8 +791,14 @@
       <c r="F5" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G5" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -706,8 +817,14 @@
       <c r="F6" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G6" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -726,8 +843,14 @@
       <c r="F7" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G7" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -743,8 +866,14 @@
       <c r="F8" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G8" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -758,77 +887,107 @@
         <v>41</v>
       </c>
       <c r="F9" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>44</v>
       </c>
       <c r="E10" s="8">
         <v>123456</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="G10" t="s">
+        <v>63</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="E11" s="8"/>
       <c r="F11" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" t="s">
+        <v>64</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="C12" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="D12" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" t="s">
+        <v>65</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="C13" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="D13" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>56</v>
       </c>
       <c r="E13" s="8"/>
       <c r="F13" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+      <c r="G13" t="s">
+        <v>66</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="peterntshuntsha24@gmail.com,07864"/>
-    <hyperlink ref="E8" r:id="rId2"/>
-    <hyperlink ref="E9" r:id="rId3" display="Peterntshuntsha24@gmail.com"/>
-    <hyperlink ref="E10" r:id="rId4" display="Peterntshuntsha24@gmail.com"/>
+    <hyperlink ref="E2" r:id="rId1" display="peterntshuntsha24@gmail.com,07864" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E8" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E9" r:id="rId3" display="Peterntshuntsha24@gmail.com" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E10" r:id="rId4" display="Peterntshuntsha24@gmail.com" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>

</xml_diff>